<commit_message>
modify v-for key why not use index
</commit_message>
<xml_diff>
--- a/js-list.xlsx
+++ b/js-list.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
   <si>
     <t>es6新特性</t>
   </si>
@@ -882,18 +887,20 @@
   <si>
     <t>通过import(*)语句来控制加载时机，webpack内置了对于import(*)的解析，会将import(*)中引入的模块作为一个新的入口在生成一个chunk。 当代码执行到import(*)语句时，会去加载Chunk对应生成的文件。import()会返回一个Promise对象，所以为了让浏览器支持，需要事先注入Promise polyfill。</t>
   </si>
+  <si>
+    <t>v-for时为什么不建议用index索引</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>当以index为索引时，如果在中间插入一条新数据，原数据插入点后的项没变化但index会递增，在虚拟dom比较新旧差异时，diff算法发现本来后几项数据也有变化，也要重新渲染，就失去了虚拟dom上的性能优势，如果用每条数据对象的某个具有唯一性的id时，即时中间插入新的数据，后面的key没有变化得到了复用，也就利用了虚拟dom的优势</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="35">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,352 +1002,35 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1348,255 +1038,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1606,112 +1054,74 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1722,7 +1132,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -1744,7 +1154,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1786,7 +1196,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1828,7 +1238,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2133,32 +1543,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="B3:G39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39:G39"/>
+      <selection activeCell="C40" sqref="C40:G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="22.5" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="22.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.975" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.475" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.1916666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="13.5" spans="2:4">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:7" ht="14">
+      <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2168,8 +1578,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="13.5" spans="2:7">
-      <c r="B4" s="3"/>
+    <row r="4" spans="2:7" ht="14">
+      <c r="B4" s="19"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2186,8 +1596,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="13.5" spans="2:7">
-      <c r="B5" s="3"/>
+    <row r="5" spans="2:7" ht="14">
+      <c r="B5" s="19"/>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2204,8 +1614,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="72" customHeight="1" spans="2:7">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:7" ht="72" customHeight="1">
+      <c r="B6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2224,8 +1634,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="13.5" spans="2:3">
-      <c r="B7" s="3"/>
+    <row r="7" spans="2:7" ht="14">
+      <c r="B7" s="19"/>
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2250,223 +1660,225 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" ht="13.5" spans="2:7">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="2:7" ht="14">
+      <c r="B10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" ht="35" customHeight="1" spans="2:7">
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" ht="13.5" spans="2:7">
-      <c r="B12" s="3" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="2:7" ht="35" customHeight="1">
+      <c r="B11" s="19"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="2:7" ht="14">
+      <c r="B12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" ht="46" customHeight="1" spans="2:7">
-      <c r="B13" s="3"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" ht="13.5" spans="2:7">
-      <c r="B14" s="3" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="2:7" ht="46" customHeight="1">
+      <c r="B13" s="19"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="2:7" ht="14">
+      <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" ht="13.5" spans="2:7">
-      <c r="B15" s="3"/>
-      <c r="C15" s="4" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="2:7" ht="14">
+      <c r="B15" s="19"/>
+      <c r="C15" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" ht="95" customHeight="1" spans="2:7">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="2:7" ht="95" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" ht="45" spans="2:4">
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="2:7" ht="42">
       <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" ht="47" customHeight="1" spans="2:4">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="2:7" ht="47" customHeight="1">
+      <c r="B18" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" ht="42" spans="2:4">
-      <c r="B19" s="3"/>
-      <c r="C19" s="8" t="s">
+    <row r="19" spans="2:7" ht="45">
+      <c r="B19" s="19"/>
+      <c r="C19" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" ht="64" customHeight="1" spans="2:6">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="2:7" ht="64" customHeight="1">
+      <c r="B20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" ht="81" customHeight="1" spans="2:6">
-      <c r="B21" s="3"/>
-      <c r="C21" s="10" t="s">
+    <row r="21" spans="2:7" ht="81" customHeight="1">
+      <c r="B21" s="19"/>
+      <c r="C21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" ht="81" customHeight="1" spans="2:7">
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="2:7" ht="81" customHeight="1">
+      <c r="B22" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" ht="130" customHeight="1" spans="3:6">
+    <row r="23" spans="2:7" ht="130" customHeight="1">
+      <c r="B23" s="20"/>
       <c r="C23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="25" spans="2:7">
       <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" ht="180" customHeight="1"/>
-    <row r="27" ht="13.5" spans="2:7">
-      <c r="B27" s="3" t="s">
+    <row r="26" spans="2:7" ht="180" customHeight="1"/>
+    <row r="27" spans="2:7" ht="14">
+      <c r="B27" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" ht="208" customHeight="1" spans="2:7">
-      <c r="B28" s="3"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" ht="57" customHeight="1" spans="2:7">
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="2:7" ht="208" customHeight="1">
+      <c r="B28" s="19"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+    </row>
+    <row r="29" spans="2:7" ht="57" customHeight="1">
       <c r="B29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" ht="43" customHeight="1" spans="2:7">
-      <c r="B30" s="3" t="s">
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="2:7" ht="43" customHeight="1">
+      <c r="B30" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" ht="58" customHeight="1" spans="3:6">
-      <c r="C31" s="16" t="s">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="2:7" ht="58" customHeight="1">
+      <c r="B31" s="20"/>
+      <c r="C31" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2479,8 +1891,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" ht="13.5" spans="2:7">
-      <c r="B32" s="3" t="s">
+    <row r="32" spans="2:7" ht="14">
+      <c r="B32" s="19" t="s">
         <v>70</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -2499,17 +1911,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" ht="100" customHeight="1" spans="2:7">
-      <c r="B33" s="3"/>
-      <c r="E33" s="10" t="s">
+    <row r="33" spans="2:7" ht="100" customHeight="1">
+      <c r="B33" s="19"/>
+      <c r="E33" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" ht="13.5" spans="2:7">
-      <c r="B34" s="3" t="s">
+    <row r="34" spans="2:7" ht="14">
+      <c r="B34" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -2528,17 +1940,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" ht="13.5" spans="2:4">
-      <c r="B35" s="3"/>
-      <c r="C35" s="17" t="s">
+    <row r="35" spans="2:7" ht="14">
+      <c r="B35" s="19"/>
+      <c r="C35" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" ht="93" spans="2:6">
-      <c r="B36" s="19" t="s">
+    <row r="36" spans="2:7" ht="84">
+      <c r="B36" s="15" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -2547,26 +1959,26 @@
       <c r="D36" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="16" t="s">
         <v>88</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" ht="156" customHeight="1" spans="2:7">
+    <row r="37" spans="2:7" ht="156" customHeight="1">
       <c r="B37" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" ht="45" spans="2:4">
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" ht="42">
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
@@ -2577,25 +1989,33 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" ht="67.5" spans="2:7">
+    <row r="39" spans="2:7" ht="42">
       <c r="B39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="2:7" ht="63">
+      <c r="B40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="C29:G29"/>
+  <mergeCells count="23">
+    <mergeCell ref="C40:G40"/>
     <mergeCell ref="C37:G37"/>
     <mergeCell ref="C39:G39"/>
     <mergeCell ref="B3:B5"/>
@@ -2612,45 +2032,59 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C12:G13"/>
     <mergeCell ref="C10:G11"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="C29:G29"/>
     <mergeCell ref="C27:G28"/>
   </mergeCells>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify vue life cycle and data return
</commit_message>
<xml_diff>
--- a/js-list.xlsx
+++ b/js-list.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="125">
   <si>
     <t>es6新特性</t>
   </si>
@@ -1528,22 +1533,64 @@
     <t>为什么需要Virtual DOM</t>
   </si>
   <si>
-    <t>首先,我们都知道在前端性能优化的一个秘诀就是尽可能少地操作DOM,不仅仅是DOM相对较慢,更因为频繁变动DOM会造成浏览器的回流或者重回,这些都是性能的杀手,因此我们需要这一层抽象,在patch过程中尽可能地一次性将差异更新到DOM中,这样保证了DOM不会出现性能很差的情况.
-其次,_x0008_现代前端框架的一个基本要求就是无须手动操作DOM,一方面是因为手动操作DOM无法保证程序性能,多人协作的项目中如果review不严格,可能会有开发者写出性能较低的代码,另一方面更重要的是省略手动DOM操作可以大大提高开发效率.
+    <t>vue路由切换，各页面的生命周期是怎样的</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入A页开始
+A-beforeCreate
+A-created
+A-beforeMount
+A-mounted
+B-beforeCreate  (开始切换B页)
+B-created
+B-beforeMount
+A-beforeDestroy
+A-destroyed
+B-mounted
+重点理解：mounted是实例被挂载后调用，所以在B页即将挂载时，A页挂载被清除(被销毁)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>vue中data数据为什么return</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>因为在vue中每个组件都是个vue实例，data数据放在函数里return出去，会有函数作用域，保证了每个组件的data数据作用域是在当前组件，不会与其他组件的共享.</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>首先,我们都知道在前端性能优化的一个秘诀就是尽可能少地操作DOM,不仅仅是DOM相对较慢,更因为频繁变动DOM会造成浏览器的回流或者重绘,这些都是性能的杀手,因此我们需要这一层抽象,在patch过程中尽可能地一次性将差异更新到DOM中,这样保证了DOM不会出现性能很差的情况.
+其次,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Marker Felt"/>
+      </rPr>
+      <t>_x0008_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>现代前端框架的一个基本要求就是无须手动操作DOM,一方面是因为手动操作DOM无法保证程序性能,多人协作的项目中如果review不严格,可能会有开发者写出性能较低的代码,另一方面更重要的是省略手动DOM操作可以大大提高开发效率.
 最后,也是Virtual DOM最初的目的,就是更好的跨平台,比如Node.js就没有DOM,如果想实现SSR(服务端渲染),那么一个方式就是借助Virtual DOM,因为Virtual DOM本身是JavaScript对象.</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="40">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1658,150 +1705,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF3E3E3E"/>
       <name val="宋体"/>
@@ -1826,202 +1729,27 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Marker Felt"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2029,255 +1757,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2290,9 +1776,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2301,9 +1784,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2322,15 +1802,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2359,58 +1830,29 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2421,7 +1863,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -2443,7 +1885,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2485,7 +1927,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2527,7 +1969,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2832,100 +2274,100 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="B3:G49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
       <selection activeCell="C49" sqref="C49:G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="22.5" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="22.1666666666667" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.8333333333333" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.1666666666667" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="26" style="3" customWidth="1"/>
     <col min="6" max="6" width="20.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="33.1666666666667" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:7" ht="17">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+    <row r="4" spans="2:7" ht="17">
+      <c r="B4" s="24"/>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="2:7" ht="17">
+      <c r="B5" s="24"/>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="72" customHeight="1" spans="2:7">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="2:7" ht="72" customHeight="1">
+      <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="2:7" ht="17">
+      <c r="B7" s="24"/>
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2933,378 +2375,380 @@
       <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:7" ht="14">
+      <c r="B10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" ht="51" customHeight="1" spans="2:7">
-      <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="4" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="2:7" ht="51" customHeight="1">
+      <c r="B11" s="24"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="2:7" ht="14">
+      <c r="B12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" ht="46" customHeight="1" spans="2:7">
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="4" t="s">
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:7" ht="46" customHeight="1">
+      <c r="B13" s="24"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="2:7" ht="17">
+      <c r="B14" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="4"/>
-      <c r="C15" s="6" t="s">
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="2:7" ht="17">
+      <c r="B15" s="24"/>
+      <c r="C15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" ht="95" customHeight="1" spans="2:7">
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="2:7" ht="95" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" ht="56.25" spans="2:4">
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="2:7" ht="51">
       <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" ht="47" customHeight="1" spans="2:4">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="2:7" ht="47" customHeight="1">
+      <c r="B18" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" ht="75" spans="2:4">
-      <c r="B19" s="4"/>
-      <c r="C19" s="11" t="s">
+    <row r="19" spans="2:7" ht="68">
+      <c r="B19" s="24"/>
+      <c r="C19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" ht="64" customHeight="1" spans="2:6">
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="2:7" ht="64" customHeight="1">
+      <c r="B20" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" ht="81" customHeight="1" spans="2:6">
-      <c r="B21" s="4"/>
-      <c r="C21" s="13" t="s">
+    <row r="21" spans="2:7" ht="81" customHeight="1">
+      <c r="B21" s="24"/>
+      <c r="C21" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" ht="81" customHeight="1" spans="2:7">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="2:7" ht="81" customHeight="1">
+      <c r="B22" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" ht="130" customHeight="1" spans="3:6">
-      <c r="C23" s="5" t="s">
+    <row r="23" spans="2:7" ht="130" customHeight="1">
+      <c r="B23" s="25"/>
+      <c r="C23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="25" spans="2:7">
       <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" ht="180" customHeight="1"/>
-    <row r="27" spans="2:7">
-      <c r="B27" s="4" t="s">
+    <row r="26" spans="2:7" ht="180" customHeight="1"/>
+    <row r="27" spans="2:7" ht="14">
+      <c r="B27" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" ht="208" customHeight="1" spans="2:7">
-      <c r="B28" s="4"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" ht="57" customHeight="1" spans="2:7">
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+    </row>
+    <row r="28" spans="2:7" ht="208" customHeight="1">
+      <c r="B28" s="24"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+    </row>
+    <row r="29" spans="2:7" ht="57" customHeight="1">
       <c r="B29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" ht="43" customHeight="1" spans="2:7">
-      <c r="B30" s="4" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+    </row>
+    <row r="30" spans="2:7" ht="43" customHeight="1">
+      <c r="B30" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" ht="58" customHeight="1" spans="3:6">
-      <c r="C31" s="18" t="s">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="2:7" ht="58" customHeight="1">
+      <c r="B31" s="25"/>
+      <c r="C31" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="4" t="s">
+    <row r="32" spans="2:7" ht="17">
+      <c r="B32" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" ht="82" customHeight="1" spans="2:7">
-      <c r="B33" s="4"/>
-      <c r="E33" s="11" t="s">
+    <row r="33" spans="2:7" ht="82" customHeight="1">
+      <c r="B33" s="24"/>
+      <c r="E33" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="4" t="s">
+    <row r="34" spans="2:7" ht="17">
+      <c r="B34" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="4"/>
-      <c r="C35" s="19" t="s">
+    <row r="35" spans="2:7" ht="17">
+      <c r="B35" s="24"/>
+      <c r="C35" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" ht="54" customHeight="1" spans="2:6">
-      <c r="B36" s="21" t="s">
+    <row r="36" spans="2:7" ht="54" customHeight="1">
+      <c r="B36" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" ht="126" customHeight="1" spans="2:7">
+    <row r="37" spans="2:7" ht="126" customHeight="1">
       <c r="B37" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" ht="45" spans="2:4">
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+    </row>
+    <row r="38" spans="2:7" ht="42">
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" ht="67.5" spans="2:7">
+    <row r="39" spans="2:7" ht="42">
       <c r="B39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" ht="67.5" spans="2:7">
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+    </row>
+    <row r="40" spans="2:7" ht="63">
       <c r="B40" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" ht="18.75" spans="2:7">
-      <c r="B41" s="4" t="s">
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+    </row>
+    <row r="41" spans="2:7" ht="17">
+      <c r="B41" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="22" t="s">
         <v>100</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -3313,26 +2757,26 @@
       <c r="E41" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G41" s="22" t="s">
+      <c r="G41" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" ht="48" spans="2:7">
-      <c r="B42" s="4"/>
-      <c r="C42" s="6"/>
-      <c r="F42" s="23" t="s">
+    <row r="42" spans="2:7" ht="36">
+      <c r="B42" s="24"/>
+      <c r="C42" s="22"/>
+      <c r="F42" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G42" s="19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="4"/>
-      <c r="C43" s="7" t="s">
+    <row r="43" spans="2:7" ht="17">
+      <c r="B43" s="24"/>
+      <c r="C43" s="22" t="s">
         <v>106</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -3342,78 +2786,108 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" ht="24" spans="2:4">
-      <c r="B44" s="4"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="23" t="s">
+    <row r="44" spans="2:7" ht="24">
+      <c r="B44" s="24"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="45" ht="13.5" spans="2:7">
-      <c r="B45" s="4" t="s">
+    <row r="45" spans="2:7" ht="14">
+      <c r="B45" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-    </row>
-    <row r="46" ht="70" customHeight="1" spans="2:7">
-      <c r="B46" s="4"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-    </row>
-    <row r="47" ht="35.25" spans="2:5">
-      <c r="B47" s="4" t="s">
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+    </row>
+    <row r="46" spans="2:7" ht="70" customHeight="1">
+      <c r="B46" s="24"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+    </row>
+    <row r="47" spans="2:7" ht="34">
+      <c r="B47" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E47" s="17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" ht="84.75" spans="2:5">
-      <c r="B48" s="4"/>
-      <c r="C48" s="25" t="s">
+    <row r="48" spans="2:7" ht="78">
+      <c r="B48" s="24"/>
+      <c r="C48" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="26" t="s">
+      <c r="D48" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E48" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="49" ht="141" customHeight="1" spans="2:7">
+    <row r="49" spans="2:7" ht="141" customHeight="1">
       <c r="B49" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+    </row>
+    <row r="50" spans="2:7" ht="221" customHeight="1">
+      <c r="B50" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
+      <c r="C50" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="23"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="2:7" ht="85" customHeight="1">
+      <c r="B51" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="23"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="C29:G29"/>
+  <mergeCells count="32">
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C12:G13"/>
+    <mergeCell ref="C10:G11"/>
+    <mergeCell ref="C27:G28"/>
+    <mergeCell ref="C45:G46"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="C37:G37"/>
     <mergeCell ref="C39:G39"/>
     <mergeCell ref="C40:G40"/>
@@ -3430,57 +2904,62 @@
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C12:G13"/>
-    <mergeCell ref="C10:G11"/>
-    <mergeCell ref="C27:G28"/>
-    <mergeCell ref="C45:G46"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="C29:G29"/>
   </mergeCells>
+  <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C48" r:id="rId2" display="vue-router配置路由，使用vue的异步组件技术，可以实现按需加载（懒加载）。 但是，这种情况下一个组件生成一个js文件。" tooltip="https://router.vuejs.org/zh-cn/advanced/lazy-loading.html"/>
-    <hyperlink ref="E48" r:id="rId3" display="vue-router配置路由，使用webpack的require.ensure技术，也可以实现按需加载。 这种情况下，多个路由指定相同的chunkName，会合并打包成一个js文件"/>
+    <hyperlink ref="C48" r:id="rId1" tooltip="https://router.vuejs.org/zh-cn/advanced/lazy-loading.html"/>
+    <hyperlink ref="E48" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify copy array and vue name
</commit_message>
<xml_diff>
--- a/js-list.xlsx
+++ b/js-list.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\resource\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6945"/>
+    <workbookView xWindow="-80" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="161">
   <si>
     <t>es6新特性</t>
   </si>
@@ -335,7 +335,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>有哪几种导航钩子</t>
@@ -347,7 +346,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>在</t>
@@ -366,7 +364,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>目录下的</t>
@@ -385,7 +382,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>文件中，对</t>
@@ -404,7 +400,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>属性加上</t>
@@ -423,7 +418,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>。</t>
@@ -443,7 +437,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>使用 router 对象的 params.id 获取</t>
@@ -470,7 +463,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>、</t>
@@ -489,7 +481,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>、</t>
@@ -508,7 +499,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>、</t>
@@ -527,7 +517,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>、</t>
@@ -559,7 +548,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>中</t>
@@ -580,7 +568,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>请求代码应该写在组件的</t>
@@ -601,7 +588,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>中还是</t>
@@ -622,7 +608,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>的</t>
@@ -643,7 +628,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>中</t>
@@ -664,7 +648,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>就是一个仓库，仓库里放了很多对象。其中</t>
@@ -683,7 +666,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>就是数据源存放地，对应于一般</t>
@@ -702,7 +684,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>对象里面的</t>
@@ -732,7 +713,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>可以对</t>
@@ -751,7 +731,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>进行计算操作，它就是</t>
@@ -770,7 +749,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>的计算属性</t>
@@ -791,7 +769,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>类似于</t>
@@ -810,7 +787,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>不同在于：</t>
@@ -829,7 +805,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>提交的是</t>
@@ -848,7 +823,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>而不是直接变更状态</t>
@@ -868,7 +842,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>可以包含任意异步操作</t>
@@ -880,7 +853,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>如果请求来的数据不是要被其他组件公用，仅仅在请求的组件内使用，就不需要放入</t>
@@ -899,7 +871,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>的</t>
@@ -918,7 +889,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>里</t>
@@ -952,7 +922,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>入口，告诉</t>
@@ -971,7 +940,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>要使用哪个模块作为构建项目的起点，默认为</t>
@@ -1012,7 +980,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>出口，告诉</t>
@@ -1031,7 +998,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>在哪里输出它打包好的代码以及如何命名，默认为</t>
@@ -1062,7 +1028,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>是用来告诉</t>
@@ -1081,7 +1046,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>如何转换某一类型的文件，并且引入到打包出的文件中。</t>
@@ -1112,7 +1076,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>插件</t>
@@ -1131,7 +1094,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>作用更大，可以打包优化，资源管理和注入环境变量</t>
@@ -1144,7 +1106,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1155,7 +1116,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1168,7 +1128,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1179,7 +1138,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1192,7 +1150,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1203,7 +1160,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1281,7 +1237,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>是</t>
@@ -1300,7 +1255,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>新引进的特性</t>
@@ -1312,7 +1266,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>服务器端对于</t>
@@ -1331,7 +1284,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>的支持，主要就是通过设置</t>
@@ -1350,7 +1302,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>来进行的。如果浏览器检测到相应的设置，就可以允许</t>
@@ -1369,7 +1320,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>进行跨域的访问</t>
@@ -1403,7 +1353,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>引用数据类型</t>
@@ -1413,7 +1362,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>：对象</t>
@@ -1432,7 +1380,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>、数组</t>
@@ -1451,7 +1398,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>、函数</t>
@@ -1470,7 +1416,6 @@
         <sz val="14"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>。</t>
@@ -1646,7 +1591,6 @@
         <sz val="11.5"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>推荐使用这种方式</t>
@@ -1665,7 +1609,6 @@
         <sz val="11.5"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>需要</t>
@@ -1685,7 +1628,6 @@
         <sz val="11.5"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>官方文档：</t>
@@ -1704,7 +1646,6 @@
         <sz val="11.5"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>中使用</t>
@@ -1723,7 +1664,6 @@
         <sz val="11.5"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>官方文档：路由懒加载使用</t>
@@ -1780,7 +1720,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1801,7 +1740,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1851,18 +1789,18 @@
     width:fit-content;
     margin:0 auto;
 }</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>.son{
     display: flex;
     justify-content: center;
 }</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>使用flex 2009年版本, 父元素display: box;box-pack: center;如下设置:</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>使用CSS3中新增的transform属性, 子元素设置如下:</t>
@@ -1873,34 +1811,219 @@
       left:50%;
       transform:translate(-50%,0);
 }</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>水平居中</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>Vue - 监听数据的三种方法</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>我们在input标签里绑定keyup事件</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>使用watch</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
     <t>computed计算属性的使用</t>
-    <phoneticPr fontId="27" type="noConversion"/>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>拷贝数组的方式</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">浅拷贝
+es6 展开运算符 (...) 可以在函数调用/数组构造时, 将数组表达式或者string在语法层面展开；还可以在构造字面量对象时, 将对象表达式按key-value的方式展开
+</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>深拷贝
+json.parse(json.stringify(arr))</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>filter 返回符合过滤条件的部分数组</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>some 只要有任意一个元素满足条件，返回 true ,否则返回 false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>every 必须全部元素满足条件，返回true，否则返回 false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>forEach 总是返回undefined</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组遍历的几张方法返回值</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>map 返回各元素是否满足条件的boolean 数组[true, false, undefined]</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>浅拷贝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+slice 方法返回一个新的数组对象，这一对象是一个由 begin 和 end 决定的原数组的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>浅拷贝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（包括 begin，不包括end）。如果该元素是个</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>对象引用 （不是实际的对象）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，slice 会拷贝这个对象引用到新的数组里。两个对象引用都引用了同一个对象。如果被引用的对象发生改变，则新的和原来的数组中的这个元素也会发生改变。元素的其他数据类型正常拷贝</t>
+    </r>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>浅拷贝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+concat 方法用于合并两个或多个数组。此方法不会更改现有数组，而是返回一个新数组. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>对象引用（而不是实际对象）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：concat将对象引用复制到新数组中。 原始数组和新数组都引用相同的对象。 也就是说，如果引用的对象被修改，则更改对于新数组和原始数组都是可见的。 这包括也是数组的数组参数的元素。元素的其他数据类型正常拷贝.</t>
+    </r>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>null 和 undefined区别</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>undefined 表示此处应该有值，但还没定义, false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>null == undefined  结果 true
+null === undefined 结果 false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>null 表示一个值被定义了，但这个值是空值 false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>vue 组件中name的用处</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. keep-alive 时用来标记组件</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 递归组件时用</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. vue 浏览器插件调试时查看组件名</t>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2048,43 +2171,12 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.5"/>
-      <color rgb="FF333333"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2131,7 +2223,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2189,8 +2281,32 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2198,33 +2314,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2657,26 +2752,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G56"/>
+  <dimension ref="B3:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="22.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="22.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="40.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="39.25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="39" style="3" customWidth="1"/>
     <col min="6" max="6" width="20.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="33.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="18.75">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:7" ht="17">
+      <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2686,8 +2781,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="18.75">
-      <c r="B4" s="20"/>
+    <row r="4" spans="2:7" ht="17">
+      <c r="B4" s="28"/>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2704,8 +2799,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="18.75">
-      <c r="B5" s="20"/>
+    <row r="5" spans="2:7" ht="17">
+      <c r="B5" s="28"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2723,7 +2818,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="72" customHeight="1">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2742,8 +2837,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="18.75">
-      <c r="B7" s="20"/>
+    <row r="7" spans="2:7" ht="17">
+      <c r="B7" s="28"/>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
@@ -2768,81 +2863,81 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="13.5">
-      <c r="B9" s="20" t="s">
+    <row r="9" spans="2:7" ht="14">
+      <c r="B9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="2:7" ht="69" customHeight="1">
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="2:7" ht="13.5">
-      <c r="B11" s="20" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="2:7" ht="14">
+      <c r="B11" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="2:7" ht="45.95" customHeight="1">
-      <c r="B12" s="20"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="2:7" ht="18.75">
-      <c r="B13" s="20" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="2:7" ht="46" customHeight="1">
+      <c r="B12" s="28"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="2:7" ht="17">
+      <c r="B13" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="2:7" ht="18.75">
-      <c r="B14" s="20"/>
-      <c r="C14" s="19" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="2:7" ht="17">
+      <c r="B14" s="28"/>
+      <c r="C14" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="2:7" ht="95.1" customHeight="1">
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="2:7" ht="95" customHeight="1">
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="2:7" ht="56.25">
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="2:7" ht="51">
       <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
@@ -2853,8 +2948,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="47.1" customHeight="1">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="2:7" ht="47" customHeight="1">
+      <c r="B17" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2864,8 +2959,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="75">
-      <c r="B18" s="20"/>
+    <row r="18" spans="2:7" ht="51">
+      <c r="B18" s="28"/>
       <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
@@ -2873,8 +2968,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="63.95" customHeight="1">
-      <c r="B19" s="20" t="s">
+    <row r="19" spans="2:7" ht="64" customHeight="1">
+      <c r="B19" s="28" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -2885,7 +2980,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="81" customHeight="1">
-      <c r="B20" s="20"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="8" t="s">
         <v>46</v>
       </c>
@@ -2900,7 +2995,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="81" customHeight="1">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="28" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2919,16 +3014,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="129.94999999999999" customHeight="1">
-      <c r="B22" s="21"/>
+    <row r="22" spans="2:7" ht="130" customHeight="1">
+      <c r="B22" s="29"/>
       <c r="C22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="2" t="s">
@@ -2936,38 +3031,38 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="180" customHeight="1"/>
-    <row r="26" spans="2:7" ht="13.5">
-      <c r="B26" s="20" t="s">
+    <row r="26" spans="2:7" ht="14">
+      <c r="B26" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="2:7" ht="207.95" customHeight="1">
-      <c r="B27" s="20"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="2:7" ht="208" customHeight="1">
+      <c r="B27" s="28"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="2:7" ht="57" customHeight="1">
       <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-    </row>
-    <row r="29" spans="2:7" ht="42.95" customHeight="1">
-      <c r="B29" s="20" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+    </row>
+    <row r="29" spans="2:7" ht="43" customHeight="1">
+      <c r="B29" s="28" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2983,8 +3078,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="57.95" customHeight="1">
-      <c r="B30" s="21"/>
+    <row r="30" spans="2:7" ht="58" customHeight="1">
+      <c r="B30" s="29"/>
       <c r="C30" s="10" t="s">
         <v>67</v>
       </c>
@@ -2998,8 +3093,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="18.75">
-      <c r="B31" s="20" t="s">
+    <row r="31" spans="2:7" ht="17">
+      <c r="B31" s="28" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -3019,7 +3114,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="96" customHeight="1">
-      <c r="B32" s="20"/>
+      <c r="B32" s="28"/>
       <c r="E32" s="6" t="s">
         <v>75</v>
       </c>
@@ -3027,8 +3122,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="18.75">
-      <c r="B33" s="20" t="s">
+    <row r="33" spans="2:7" ht="17">
+      <c r="B33" s="28" t="s">
         <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -3047,8 +3142,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="37.5">
-      <c r="B34" s="20"/>
+    <row r="34" spans="2:7" ht="34">
+      <c r="B34" s="28"/>
       <c r="C34" s="11" t="s">
         <v>83</v>
       </c>
@@ -3077,15 +3172,15 @@
       <c r="B36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-    </row>
-    <row r="37" spans="2:7" ht="45">
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+    </row>
+    <row r="37" spans="2:7" ht="42">
       <c r="B37" s="2" t="s">
         <v>92</v>
       </c>
@@ -3096,35 +3191,35 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="67.5">
+    <row r="38" spans="2:7" ht="42">
       <c r="B38" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-    </row>
-    <row r="39" spans="2:7" ht="67.5">
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+    </row>
+    <row r="39" spans="2:7" ht="63">
       <c r="B39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-    </row>
-    <row r="40" spans="2:7" ht="18.75">
-      <c r="B40" s="20" t="s">
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+    </row>
+    <row r="40" spans="2:7" ht="17">
+      <c r="B40" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="25" t="s">
         <v>100</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -3140,9 +3235,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="48">
-      <c r="B41" s="20"/>
-      <c r="C41" s="19"/>
+    <row r="41" spans="2:7" ht="36">
+      <c r="B41" s="28"/>
+      <c r="C41" s="25"/>
       <c r="F41" s="15" t="s">
         <v>104</v>
       </c>
@@ -3150,9 +3245,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="18.75">
-      <c r="B42" s="20"/>
-      <c r="C42" s="19" t="s">
+    <row r="42" spans="2:7" ht="17">
+      <c r="B42" s="28"/>
+      <c r="C42" s="25" t="s">
         <v>106</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -3163,34 +3258,34 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="24">
-      <c r="B43" s="20"/>
-      <c r="C43" s="19"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="13.5">
-      <c r="B44" s="20" t="s">
+    <row r="44" spans="2:7" ht="14">
+      <c r="B44" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-    </row>
-    <row r="45" spans="2:7" ht="69.95" customHeight="1">
-      <c r="B45" s="20"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-    </row>
-    <row r="46" spans="2:7" ht="18.75">
-      <c r="B46" s="20" t="s">
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+    </row>
+    <row r="45" spans="2:7" ht="70" customHeight="1">
+      <c r="B45" s="28"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+    </row>
+    <row r="46" spans="2:7" ht="17">
+      <c r="B46" s="28" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="14" t="s">
@@ -3203,8 +3298,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="2:7" ht="57">
-      <c r="B47" s="20"/>
+    <row r="47" spans="2:7" ht="52">
+      <c r="B47" s="28"/>
       <c r="C47" s="17" t="s">
         <v>116</v>
       </c>
@@ -3215,8 +3310,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="2:7" ht="175.5">
-      <c r="B48" s="20"/>
+    <row r="48" spans="2:7" ht="180">
+      <c r="B48" s="28"/>
       <c r="C48" s="17" t="s">
         <v>119</v>
       </c>
@@ -3231,100 +3326,177 @@
       <c r="B49" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="2:7" ht="221.1" customHeight="1">
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+    </row>
+    <row r="50" spans="2:7" ht="221" customHeight="1">
       <c r="B50" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="D50" s="19"/>
-    </row>
-    <row r="51" spans="2:7" ht="84.95" customHeight="1">
+      <c r="D50" s="25"/>
+    </row>
+    <row r="51" spans="2:7" ht="85" customHeight="1">
       <c r="B51" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="19"/>
-    </row>
-    <row r="52" spans="2:7" ht="56.25">
-      <c r="B52" s="29" t="s">
+      <c r="D51" s="25"/>
+    </row>
+    <row r="52" spans="2:7" ht="51">
+      <c r="B52" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="D52" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="26" t="s">
+      <c r="E52" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F52" s="26" t="s">
+      <c r="F52" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="G52" s="27" t="s">
+      <c r="G52" s="22" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="131.25">
-      <c r="B53" s="29"/>
-      <c r="E53" s="27" t="s">
+    <row r="53" spans="2:7" ht="102">
+      <c r="B53" s="27"/>
+      <c r="E53" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="F53" s="27" t="s">
+      <c r="F53" s="22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="28.5">
-      <c r="B54" s="29"/>
-      <c r="C54" s="26" t="s">
+    <row r="54" spans="2:7" ht="26">
+      <c r="B54" s="27"/>
+      <c r="C54" s="21" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="60">
-      <c r="B55" s="29"/>
-      <c r="C55" s="28" t="s">
+      <c r="B55" s="27"/>
+      <c r="C55" s="23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="45">
-      <c r="B56" s="24" t="s">
+    <row r="56" spans="2:7" ht="42">
+      <c r="B56" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="27" t="s">
+      <c r="D56" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="E56" s="27" t="s">
+      <c r="E56" s="22" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="187">
+      <c r="B57" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="68">
+      <c r="B58" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="42">
+      <c r="B59" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="42">
+      <c r="B60" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="C11:G12"/>
     <mergeCell ref="C9:G10"/>
     <mergeCell ref="C26:G27"/>
     <mergeCell ref="C44:G45"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="C51:D51"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B21:B22"/>
@@ -3335,20 +3507,8 @@
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="C28:G28"/>
   </mergeCells>
-  <phoneticPr fontId="27" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C47" r:id="rId1" tooltip="https://router.vuejs.org/zh-cn/advanced/lazy-loading.html"/>
     <hyperlink ref="E47" r:id="rId2"/>
@@ -3356,6 +3516,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3365,11 +3530,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
-  <phoneticPr fontId="27" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3379,10 +3549,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
-  <phoneticPr fontId="27" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify extend and between objects is same
</commit_message>
<xml_diff>
--- a/js-list.xlsx
+++ b/js-list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="172">
   <si>
     <t>es6新特性</t>
   </si>
@@ -1494,35 +1494,6 @@
   </si>
   <si>
     <t>递归拷贝</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF333333"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">const </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF0086B3"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>clone</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF333333"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Person = JSON.parse(JSON.stringify(person))</t>
-    </r>
   </si>
   <si>
     <t>什么是saas系统</t>
@@ -1844,178 +1815,296 @@
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
+    <t>filter 返回符合过滤条件的部分数组</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>some 只要有任意一个元素满足条件，返回 true ,否则返回 false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>every 必须全部元素满足条件，返回true，否则返回 false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>forEach 总是返回undefined</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>map 返回各元素是否满足条件的boolean 数组[true, false, undefined]</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>浅拷贝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+slice 方法返回一个新的数组对象，这一对象是一个由 begin 和 end 决定的原数组的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>浅拷贝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（包括 begin，不包括end）。如果该元素是个</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>对象引用 （不是实际的对象）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，slice 会拷贝这个对象引用到新的数组里。两个对象引用都引用了同一个对象。如果被引用的对象发生改变，则新的和原来的数组中的这个元素也会发生改变。元素的其他数据类型正常拷贝</t>
+    </r>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>浅拷贝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+concat 方法用于合并两个或多个数组。此方法不会更改现有数组，而是返回一个新数组. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>对象引用（而不是实际对象）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：concat将对象引用复制到新数组中。 原始数组和新数组都引用相同的对象。 也就是说，如果引用的对象被修改，则更改对于新数组和原始数组都是可见的。 这包括也是数组的数组参数的元素。元素的其他数据类型正常拷贝.</t>
+    </r>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>null 和 undefined区别</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>vue 组件中name的用处</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. keep-alive 时用来标记组件</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. vue 浏览器插件调试时查看组件名</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>null == undefined  结果 true
+null === undefined 结果 false</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>null 表示'没有值' 即该处不应该有值
+Number(null) 为 数字0</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>undefined 表示'缺少值'此处应该有值，但还没定义. Number(undefined) 为 NaN</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 递归组件时可用</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>js 构造函数继承的几种方式</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>http和https区别</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>tcp三次握手</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>性能优化</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
     <t>深拷贝
 json.parse(json.stringify(arr))</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
-    <t>filter 返回符合过滤条件的部分数组</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>some 只要有任意一个元素满足条件，返回 true ,否则返回 false</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>every 必须全部元素满足条件，返回true，否则返回 false</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>forEach 总是返回undefined</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>数组遍历的几张方法返回值</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>map 返回各元素是否满足条件的boolean 数组[true, false, undefined]</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>浅拷贝</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-slice 方法返回一个新的数组对象，这一对象是一个由 begin 和 end 决定的原数组的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>浅拷贝</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（包括 begin，不包括end）。如果该元素是个</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>对象引用 （不是实际的对象）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>，slice 会拷贝这个对象引用到新的数组里。两个对象引用都引用了同一个对象。如果被引用的对象发生改变，则新的和原来的数组中的这个元素也会发生改变。元素的其他数据类型正常拷贝</t>
-    </r>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>浅拷贝</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-concat 方法用于合并两个或多个数组。此方法不会更改现有数组，而是返回一个新数组. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>对象引用（而不是实际对象）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>：concat将对象引用复制到新数组中。 原始数组和新数组都引用相同的对象。 也就是说，如果引用的对象被修改，则更改对于新数组和原始数组都是可见的。 这包括也是数组的数组参数的元素。元素的其他数据类型正常拷贝.</t>
-    </r>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>null 和 undefined区别</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>undefined 表示此处应该有值，但还没定义, false</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>null == undefined  结果 true
-null === undefined 结果 false</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>null 表示一个值被定义了，但这个值是空值 false</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>vue 组件中name的用处</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. keep-alive 时用来标记组件</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 递归组件时用</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. vue 浏览器插件调试时查看组件名</t>
+    <r>
+      <t xml:space="preserve">const </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0086B3"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>clone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Person = JSON.parse(JSON.stringify(person))
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>缺点：value是function或undefined 不能拷贝</t>
+    </r>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>let obj1 = {
+  arr: [
+    {
+      prop: 1,
+    },
+    {
+      prop: 2,
+    },
+  ],
+};
+function copy(obj) {
+  var newObj = obj instanceof Array &amp;&amp; [] || {};
+  for(let key in obj) {
+    newObj[key] = obj[key] instanceof Object &amp;&amp; copy(obj[key]) || obj[key];  
+  }
+  return newObj;
+}</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>原型链继承
+child.prototype = new parent();
+缺点：
+1.对于数组，对象这些按引用路径赋值的属性会被所有实例共享.
+2.创建child实例时，无法向parent传参数</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">借助构造函数
+function Parent() {
+  this.name = ['Dav', 'Li'];
+}
+function Child() {
+  Parent.call(this);
+}
+var child1 = new Child('Davio');
+var child2 = new Child('James');
+优点：
+1. 避免引用类型值被全部实例共享.
+2. Child时可以向Parent传参.
+缺点：
+1. 方法都在构造函数中定义，每次实例都要创建一遍方法.
+</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>浏览器 (能听到我说话吗)-&gt;  服务器
+浏览器 &lt;- (可以 能听到我说话吗) 服务器
+浏览器 (我也能听到，开始连接) -&gt;  服务器</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>cors跨域的原理</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组遍历方法返回值</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断两个对象相等</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>var a = {a: 1, b: [2,5]};
+var b = {a: 2, b: [5,2]};
+console.log(JSON.stringify(a) == JSON.stringify(b));</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
 </sst>
@@ -2023,7 +2112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2200,6 +2289,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2296,10 +2392,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2309,13 +2411,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2752,10 +2848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G60"/>
+  <dimension ref="B3:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0"/>
@@ -2771,7 +2867,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="17">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2782,7 +2878,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="17">
-      <c r="B4" s="28"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2800,7 +2896,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="17">
-      <c r="B5" s="28"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2818,7 +2914,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="72" customHeight="1">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2838,7 +2934,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="17">
-      <c r="B7" s="28"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
@@ -2864,7 +2960,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="14">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="25" t="s">
@@ -2876,7 +2972,7 @@
       <c r="G9" s="25"/>
     </row>
     <row r="10" spans="2:7" ht="69" customHeight="1">
-      <c r="B10" s="28"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -2884,27 +2980,27 @@
       <c r="G10" s="25"/>
     </row>
     <row r="11" spans="2:7" ht="14">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="2:7" ht="46" customHeight="1">
-      <c r="B12" s="28"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="2:7" ht="17">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="25" t="s">
@@ -2916,7 +3012,7 @@
       <c r="G13" s="25"/>
     </row>
     <row r="14" spans="2:7" ht="17">
-      <c r="B14" s="28"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="25" t="s">
         <v>32</v>
       </c>
@@ -2949,7 +3045,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="47" customHeight="1">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2960,7 +3056,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="51">
-      <c r="B18" s="28"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
@@ -2969,7 +3065,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="64" customHeight="1">
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -2980,7 +3076,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="81" customHeight="1">
-      <c r="B20" s="28"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="8" t="s">
         <v>46</v>
       </c>
@@ -2995,7 +3091,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="81" customHeight="1">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="26" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -3015,7 +3111,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="130" customHeight="1">
-      <c r="B22" s="29"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="3" t="s">
         <v>56</v>
       </c>
@@ -3032,22 +3128,22 @@
     </row>
     <row r="25" spans="2:7" ht="180" customHeight="1"/>
     <row r="26" spans="2:7" ht="14">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="2:7" ht="208" customHeight="1">
-      <c r="B27" s="28"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="2:7" ht="57" customHeight="1">
       <c r="B28" s="2" t="s">
@@ -3062,7 +3158,7 @@
       <c r="G28" s="25"/>
     </row>
     <row r="29" spans="2:7" ht="43" customHeight="1">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -3079,7 +3175,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="58" customHeight="1">
-      <c r="B30" s="29"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="10" t="s">
         <v>67</v>
       </c>
@@ -3094,7 +3190,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="17">
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="26" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -3114,7 +3210,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="96" customHeight="1">
-      <c r="B32" s="28"/>
+      <c r="B32" s="26"/>
       <c r="E32" s="6" t="s">
         <v>75</v>
       </c>
@@ -3123,7 +3219,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="17">
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -3143,7 +3239,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="34">
-      <c r="B34" s="28"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="11" t="s">
         <v>83</v>
       </c>
@@ -3216,7 +3312,7 @@
       <c r="G39" s="25"/>
     </row>
     <row r="40" spans="2:7" ht="17">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="26" t="s">
         <v>99</v>
       </c>
       <c r="C40" s="25" t="s">
@@ -3236,7 +3332,7 @@
       </c>
     </row>
     <row r="41" spans="2:7" ht="36">
-      <c r="B41" s="28"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="25"/>
       <c r="F41" s="15" t="s">
         <v>104</v>
@@ -3246,7 +3342,7 @@
       </c>
     </row>
     <row r="42" spans="2:7" ht="17">
-      <c r="B42" s="28"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="25" t="s">
         <v>106</v>
       </c>
@@ -3257,19 +3353,22 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="24">
-      <c r="B43" s="28"/>
+    <row r="43" spans="2:7" ht="340">
+      <c r="B43" s="26"/>
       <c r="C43" s="25"/>
       <c r="D43" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="14">
+      <c r="B44" s="26" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" ht="14">
-      <c r="B44" s="28" t="s">
+      <c r="C44" s="25" t="s">
         <v>110</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>111</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
@@ -3277,7 +3376,7 @@
       <c r="G44" s="25"/>
     </row>
     <row r="45" spans="2:7" ht="70" customHeight="1">
-      <c r="B45" s="28"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="25"/>
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
@@ -3285,49 +3384,49 @@
       <c r="G45" s="25"/>
     </row>
     <row r="46" spans="2:7" ht="17">
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="D46" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="E46" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E46" s="14" t="s">
+    </row>
+    <row r="47" spans="2:7" ht="52">
+      <c r="B47" s="26"/>
+      <c r="C47" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" ht="52">
-      <c r="B47" s="28"/>
-      <c r="C47" s="17" t="s">
+      <c r="D47" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="E47" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E47" s="17" t="s">
+    </row>
+    <row r="48" spans="2:7" ht="180">
+      <c r="B48" s="26"/>
+      <c r="C48" s="17" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" ht="180">
-      <c r="B48" s="28"/>
-      <c r="C48" s="17" t="s">
+      <c r="D48" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="E48" s="17" t="s">
         <v>120</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="141" customHeight="1">
       <c r="B49" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>123</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
@@ -3336,161 +3435,186 @@
     </row>
     <row r="50" spans="2:7" ht="221" customHeight="1">
       <c r="B50" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="25" t="s">
         <v>124</v>
-      </c>
-      <c r="C50" s="25" t="s">
-        <v>125</v>
       </c>
       <c r="D50" s="25"/>
     </row>
     <row r="51" spans="2:7" ht="85" customHeight="1">
       <c r="B51" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="D51" s="25"/>
+    </row>
+    <row r="52" spans="2:7" ht="51">
+      <c r="B52" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="25"/>
-    </row>
-    <row r="52" spans="2:7" ht="51">
-      <c r="B52" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" s="21" t="s">
+      <c r="D52" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="D52" s="20" t="s">
+      <c r="E52" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="F52" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="G52" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="102">
+      <c r="B53" s="29"/>
+      <c r="E53" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="G52" s="22" t="s">
+      <c r="F53" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="26">
+      <c r="B54" s="29"/>
+      <c r="C54" s="21" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="102">
-      <c r="B53" s="27"/>
-      <c r="E53" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="F53" s="22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="26">
-      <c r="B54" s="27"/>
-      <c r="C54" s="21" t="s">
+    <row r="55" spans="2:7" ht="60">
+      <c r="B55" s="29"/>
+      <c r="C55" s="23" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="60">
-      <c r="B55" s="27"/>
-      <c r="C55" s="23" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="42">
       <c r="B56" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="D56" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="E56" s="22" t="s">
         <v>140</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="187">
       <c r="B57" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E57" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D57" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="E57" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="F57" s="30" t="s">
-        <v>144</v>
+      <c r="F57" s="24" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="68">
       <c r="B58" s="2" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="51">
+      <c r="B59" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="42">
-      <c r="B59" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="C59" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="60" spans="2:7" ht="42">
       <c r="B60" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="E60" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="323">
+      <c r="B61" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="C61" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="42">
+      <c r="B62" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E60" s="3" t="s">
+    </row>
+    <row r="63" spans="2:7" ht="85">
+      <c r="B63" s="2" t="s">
         <v>160</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="B64" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="68">
+      <c r="B66" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="C11:G12"/>
     <mergeCell ref="C9:G10"/>
     <mergeCell ref="C26:G27"/>
@@ -3507,6 +3631,23 @@
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="C28:G28"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
modify js extends of group
</commit_message>
<xml_diff>
--- a/js-list.xlsx
+++ b/js-list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="174">
   <si>
     <t>es6新特性</t>
   </si>
@@ -2066,45 +2066,83 @@
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
+    <t>浏览器 (能听到我说话吗)-&gt;  服务器
+浏览器 &lt;- (可以 能听到我说话吗) 服务器
+浏览器 (我也能听到，开始连接) -&gt;  服务器</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>cors跨域的原理</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组遍历方法返回值</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断两个对象相等</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>var a = {a: 1, b: [2,5]};
+var b = {a: 2, b: [5,2]};
+console.log(JSON.stringify(a) == JSON.stringify(b));</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">借助构造函数
 function Parent() {
   this.name = ['Dav', 'Li'];
+}
+Parent.prototype.getName = function() {
+  console.log(this.name);
 }
 function Child() {
   Parent.call(this);
 }
 var child1 = new Child('Davio');
 var child2 = new Child('James');
+child1.getName();  //Error
 优点：
 1. 避免引用类型值被全部实例共享.
 2. Child时可以向Parent传参.
 缺点：
-1. 方法都在构造函数中定义，每次实例都要创建一遍方法.
+1. 不能继承到构造函数原型上的方法，只能继承到定义在构造函数的方法，每次实例都要创建一遍方法.
 </t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
-    <t>浏览器 (能听到我说话吗)-&gt;  服务器
-浏览器 &lt;- (可以 能听到我说话吗) 服务器
-浏览器 (我也能听到，开始连接) -&gt;  服务器</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>cors跨域的原理</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>数组遍历方法返回值</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>判断两个对象相等</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>var a = {a: 1, b: [2,5]};
-var b = {a: 2, b: [5,2]};
-console.log(JSON.stringify(a) == JSON.stringify(b));</t>
+    <t xml:space="preserve">组合继承
+原型链继承和借助构造函数继承的组合
+function Parent(name) {
+  this.name = name;
+  this.colors = ['pink', 'blue'];
+}
+Parent.prototype.getName = function() {
+  console.log(this.name);
+}
+function Child(name, age) {
+  Parent.call(this, name);
+  this.age = age;
+}
+Child.prototype = new Parent();
+Child.prototype.constructor = Child;
+var child1 = new Child('Devin', 18);
+var child2 = new Child('Yioo', 20);
+child1.colors.push('black');
+console.log(child1.colors)
+console.log(child2.colors);
+child1.getName();
+child2.getName();
+优点：融合原型链和借助的优点，是JS中最常用的模式.
+缺点：调用两次父构造函数
+  第一次在Child.prototype = new Parent()
+  第二次在var child1 = new Child(); 在new Child()，回想下new模拟实现，会执行 Parent.call(this); 
+</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>new 模拟实现</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
 </sst>
@@ -2395,19 +2433,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2848,10 +2886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G66"/>
+  <dimension ref="B3:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0"/>
@@ -2867,7 +2905,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="17">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2878,7 +2916,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="17">
-      <c r="B4" s="26"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2896,7 +2934,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="17">
-      <c r="B5" s="26"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2914,7 +2952,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="72" customHeight="1">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2934,7 +2972,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="17">
-      <c r="B7" s="26"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
@@ -2960,78 +2998,78 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="14">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="2:7" ht="69" customHeight="1">
-      <c r="B10" s="26"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="2:7" ht="14">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="2:7" ht="46" customHeight="1">
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="2:7" ht="17">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="2:7" ht="17">
-      <c r="B14" s="26"/>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="2:7" ht="95" customHeight="1">
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="2:7" ht="51">
       <c r="B16" s="2" t="s">
@@ -3045,7 +3083,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="47" customHeight="1">
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -3056,7 +3094,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="51">
-      <c r="B18" s="26"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
@@ -3065,7 +3103,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="64" customHeight="1">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="29" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -3076,7 +3114,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="81" customHeight="1">
-      <c r="B20" s="26"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="8" t="s">
         <v>46</v>
       </c>
@@ -3091,7 +3129,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="81" customHeight="1">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="29" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -3115,11 +3153,11 @@
       <c r="C22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="2" t="s">
@@ -3128,37 +3166,37 @@
     </row>
     <row r="25" spans="2:7" ht="180" customHeight="1"/>
     <row r="26" spans="2:7" ht="14">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="2:7" ht="208" customHeight="1">
-      <c r="B27" s="26"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="2:7" ht="57" customHeight="1">
       <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="2:7" ht="43" customHeight="1">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="29" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -3190,7 +3228,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="17">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="29" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -3210,7 +3248,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="96" customHeight="1">
-      <c r="B32" s="26"/>
+      <c r="B32" s="29"/>
       <c r="E32" s="6" t="s">
         <v>75</v>
       </c>
@@ -3219,7 +3257,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="17">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="29" t="s">
         <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -3239,7 +3277,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="34">
-      <c r="B34" s="26"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="11" t="s">
         <v>83</v>
       </c>
@@ -3268,13 +3306,13 @@
       <c r="B36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="2:7" ht="42">
       <c r="B37" s="2" t="s">
@@ -3291,31 +3329,31 @@
       <c r="B38" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="2:7" ht="63">
       <c r="B39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="2:7" ht="17">
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="26" t="s">
         <v>100</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -3332,8 +3370,8 @@
       </c>
     </row>
     <row r="41" spans="2:7" ht="36">
-      <c r="B41" s="26"/>
-      <c r="C41" s="25"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="26"/>
       <c r="F41" s="15" t="s">
         <v>104</v>
       </c>
@@ -3342,8 +3380,8 @@
       </c>
     </row>
     <row r="42" spans="2:7" ht="17">
-      <c r="B42" s="26"/>
-      <c r="C42" s="25" t="s">
+      <c r="B42" s="29"/>
+      <c r="C42" s="26" t="s">
         <v>106</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -3354,8 +3392,8 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="340">
-      <c r="B43" s="26"/>
-      <c r="C43" s="25"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="26"/>
       <c r="D43" s="15" t="s">
         <v>163</v>
       </c>
@@ -3364,27 +3402,27 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="14">
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
     </row>
     <row r="45" spans="2:7" ht="70" customHeight="1">
-      <c r="B45" s="26"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
     </row>
     <row r="46" spans="2:7" ht="17">
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="29" t="s">
         <v>111</v>
       </c>
       <c r="C46" s="14" t="s">
@@ -3398,7 +3436,7 @@
       </c>
     </row>
     <row r="47" spans="2:7" ht="52">
-      <c r="B47" s="26"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="17" t="s">
         <v>115</v>
       </c>
@@ -3410,7 +3448,7 @@
       </c>
     </row>
     <row r="48" spans="2:7" ht="180">
-      <c r="B48" s="26"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="17" t="s">
         <v>118</v>
       </c>
@@ -3425,34 +3463,34 @@
       <c r="B49" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
     </row>
     <row r="50" spans="2:7" ht="221" customHeight="1">
       <c r="B50" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D50" s="25"/>
+      <c r="D50" s="26"/>
     </row>
     <row r="51" spans="2:7" ht="85" customHeight="1">
       <c r="B51" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="D51" s="25"/>
+      <c r="D51" s="26"/>
     </row>
     <row r="52" spans="2:7" ht="51">
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="28" t="s">
         <v>136</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -3472,7 +3510,7 @@
       </c>
     </row>
     <row r="53" spans="2:7" ht="102">
-      <c r="B53" s="29"/>
+      <c r="B53" s="28"/>
       <c r="E53" s="22" t="s">
         <v>131</v>
       </c>
@@ -3481,13 +3519,13 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="26">
-      <c r="B54" s="29"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="21" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="60">
-      <c r="B55" s="29"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="23" t="s">
         <v>135</v>
       </c>
@@ -3525,7 +3563,7 @@
     </row>
     <row r="58" spans="2:7" ht="68">
       <c r="B58" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>147</v>
@@ -3571,7 +3609,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="61" spans="2:7" ht="323">
+    <row r="61" spans="2:7" ht="409">
       <c r="B61" s="2" t="s">
         <v>158</v>
       </c>
@@ -3579,7 +3617,10 @@
         <v>165</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>166</v>
+        <v>171</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="2:7" ht="42">
@@ -3592,7 +3633,7 @@
         <v>160</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -3602,19 +3643,41 @@
     </row>
     <row r="65" spans="2:3">
       <c r="B65" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="68">
       <c r="B66" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>171</v>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="C11:G12"/>
     <mergeCell ref="C9:G10"/>
     <mergeCell ref="C26:G27"/>
@@ -3631,23 +3694,6 @@
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B46:B48"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="C28:G28"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>

</xml_diff>